<commit_message>
updated wxDC files and .xlxs file
</commit_message>
<xml_diff>
--- a/Navigator Performance Testing.xlsx
+++ b/Navigator Performance Testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>wxDC (w/ GraphicsContext)</t>
   </si>
@@ -24,37 +24,13 @@
     <t>FloatCanvas</t>
   </si>
   <si>
-    <t>OGL</t>
-  </si>
-  <si>
     <t>Pygame (w/ wx)</t>
   </si>
   <si>
-    <t>Drawing 3000 Rects (w/ Text)</t>
+    <t>17.5099999905  seconds</t>
   </si>
   <si>
-    <t>Moving Rects on canvas (w/ 3000 rects)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawing 500 Rects (w/text) </t>
-  </si>
-  <si>
-    <t>0.0620000362396 seconds</t>
-  </si>
-  <si>
-    <t>0.0160000324249 seconds</t>
-  </si>
-  <si>
-    <t>0.138999938965 Seconds</t>
-  </si>
-  <si>
-    <t>0.598999977112 Seconds</t>
-  </si>
-  <si>
-    <t>0.147000074387  seconds</t>
-  </si>
-  <si>
-    <t>0.0469999313354  seconds</t>
+    <t>ReDrawing 2500 Rects (w/text) 100 times</t>
   </si>
 </sst>
 </file>
@@ -402,50 +378,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -454,18 +418,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated performance excel file
</commit_message>
<xml_diff>
--- a/Navigator Performance Testing.xlsx
+++ b/Navigator Performance Testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>wxDC (w/ GraphicsContext)</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>ReDrawing 2500 Rects (w/text) 100 times</t>
+  </si>
+  <si>
+    <t>8.81100010872 Seconds</t>
+  </si>
+  <si>
+    <t>194.180000000 seconds</t>
   </si>
 </sst>
 </file>
@@ -381,7 +387,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,10 +417,16 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed some stuff in FloatCanvas and added some optimizations
</commit_message>
<xml_diff>
--- a/Navigator Performance Testing.xlsx
+++ b/Navigator Performance Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="19140" windowHeight="11112"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19140" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,15 +381,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -418,11 +418,11 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>194.18</v>
+        <v>75.9709</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C4" si="0">B3/100</f>
-        <v>1.9418</v>
+        <v>0.75970899999999997</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -452,7 +452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -464,7 +464,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>